<commit_message>
Modify the circuit in order to fit with the UGV v2.0 wiring
</commit_message>
<xml_diff>
--- a/fuel-gauge/Bill-Of-Materials-fuel-gauge.xlsx
+++ b/fuel-gauge/Bill-Of-Materials-fuel-gauge.xlsx
@@ -382,7 +382,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -515,19 +515,6 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -539,6 +526,45 @@
         <color indexed="64"/>
       </right>
       <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -551,7 +577,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -580,130 +606,142 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1010,8 +1048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1033,18 +1071,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="50"/>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
+      <c r="A1" s="27"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
       <c r="J1" s="4"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="50"/>
+      <c r="A2" s="27"/>
       <c r="B2" s="8" t="s">
         <v>33</v>
       </c>
@@ -1060,615 +1098,605 @@
       <c r="F2" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
       <c r="J2" s="4"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="50"/>
-      <c r="B3" s="10" t="s">
+      <c r="A3" s="27"/>
+      <c r="B3" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="11"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
       <c r="J3" s="4"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="50"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="14" t="s">
+      <c r="A4" s="27"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="15"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="50"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
       <c r="J4" s="4"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="50"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="17" t="s">
+      <c r="A5" s="27"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="50"/>
-      <c r="H5" s="50"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
       <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="50"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="17" t="s">
+      <c r="A6" s="27"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="50"/>
-      <c r="H6" s="50"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
       <c r="J6" s="4"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="50"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="20" t="s">
+      <c r="A7" s="27"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
       <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="50"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="11" t="s">
+      <c r="A8" s="27"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="11"/>
-      <c r="G8" s="50"/>
-      <c r="H8" s="50"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
       <c r="J8" s="4"/>
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="50"/>
-      <c r="B9" s="24" t="s">
+      <c r="A9" s="27"/>
+      <c r="B9" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="E9" s="26" t="s">
+      <c r="E9" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="F9" s="25"/>
-      <c r="G9" s="50"/>
-      <c r="H9" s="50"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
       <c r="J9" s="4"/>
     </row>
     <row r="10" spans="1:10" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="50"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="11" t="s">
+      <c r="A10" s="27"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="11" t="s">
+      <c r="E10" s="11"/>
+      <c r="F10" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="G10" s="50"/>
-      <c r="H10" s="50"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
       <c r="J10" s="6"/>
     </row>
     <row r="11" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="50"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="14" t="s">
+      <c r="A11" s="27"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="15"/>
-      <c r="G11" s="50"/>
-      <c r="H11" s="50"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
       <c r="J11" s="6"/>
     </row>
     <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="50"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="20" t="s">
+      <c r="A12" s="27"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="21"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="50"/>
-      <c r="H12" s="50"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
       <c r="J12" s="4"/>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="50"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="11" t="s">
+      <c r="A13" s="27"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="11"/>
-      <c r="G13" s="50"/>
-      <c r="H13" s="50"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
       <c r="J13" s="4"/>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="50"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="25" t="s">
+      <c r="A14" s="27"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="25" t="s">
+      <c r="D14" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="E14" s="26" t="s">
+      <c r="E14" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="F14" s="25"/>
-      <c r="G14" s="50"/>
-      <c r="H14" s="50"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
       <c r="J14" s="4"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="50"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="28" t="s">
+      <c r="A15" s="27"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="29" t="s">
+      <c r="D15" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="E15" s="30" t="s">
+      <c r="E15" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="29"/>
-      <c r="G15" s="50"/>
-      <c r="H15" s="50"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
       <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="50"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="31" t="s">
+      <c r="A16" s="27"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="D16" s="32"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="50"/>
-      <c r="H16" s="50"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
       <c r="J16" s="4"/>
     </row>
     <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="50"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="34" t="s">
+      <c r="A17" s="27"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="35"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="50"/>
-      <c r="H17" s="50"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
       <c r="J17" s="4"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="50"/>
-      <c r="B18" s="37"/>
-      <c r="C18" s="38" t="s">
+      <c r="A18" s="27"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="E18" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="15"/>
-      <c r="G18" s="50"/>
-      <c r="H18" s="50"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
       <c r="J18" s="4"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="50"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="39" t="s">
+      <c r="A19" s="27"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="D19" s="18"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="50"/>
-      <c r="H19" s="50"/>
+      <c r="D19" s="53"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
       <c r="J19" s="4"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="50"/>
-      <c r="B20" s="37"/>
-      <c r="C20" s="17" t="s">
+      <c r="A20" s="27"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="D20" s="18"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="50"/>
-      <c r="H20" s="50"/>
+      <c r="D20" s="53"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="39"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
       <c r="J20" s="4"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="50"/>
-      <c r="B21" s="37"/>
-      <c r="C21" s="17" t="s">
+      <c r="A21" s="27"/>
+      <c r="B21" s="49"/>
+      <c r="C21" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="D21" s="18"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="50"/>
-      <c r="H21" s="50"/>
+      <c r="D21" s="53"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
       <c r="J21" s="4"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="50"/>
-      <c r="B22" s="37"/>
-      <c r="C22" s="17" t="s">
+      <c r="A22" s="27"/>
+      <c r="B22" s="49"/>
+      <c r="C22" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="D22" s="18"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="50"/>
-      <c r="H22" s="50"/>
+      <c r="D22" s="53"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
       <c r="J22" s="4"/>
       <c r="L22" s="5"/>
     </row>
     <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="50"/>
-      <c r="B23" s="37"/>
-      <c r="C23" s="20" t="s">
+      <c r="A23" s="27"/>
+      <c r="B23" s="49"/>
+      <c r="C23" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="D23" s="21"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="50"/>
-      <c r="H23" s="50"/>
+      <c r="D23" s="55"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
       <c r="J23" s="4"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="50"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="11" t="s">
+      <c r="A24" s="27"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="D24" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="E24" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="F24" s="11"/>
-      <c r="G24" s="50"/>
-      <c r="H24" s="50"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="27"/>
       <c r="J24" s="4"/>
     </row>
     <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="50"/>
-      <c r="B25" s="27"/>
-      <c r="C25" s="25" t="s">
+      <c r="A25" s="27"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="D25" s="25" t="s">
+      <c r="D25" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="E25" s="26"/>
-      <c r="F25" s="25" t="s">
+      <c r="E25" s="18"/>
+      <c r="F25" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="G25" s="50"/>
-      <c r="H25" s="50"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="27"/>
       <c r="J25" s="4"/>
       <c r="M25" s="7"/>
     </row>
     <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="50"/>
-      <c r="B26" s="40"/>
-      <c r="C26" s="11" t="s">
+      <c r="A26" s="27"/>
+      <c r="B26" s="30"/>
+      <c r="C26" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D26" s="11" t="s">
+      <c r="D26" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="E26" s="11" t="s">
+      <c r="E26" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F26" s="11"/>
-      <c r="G26" s="50"/>
-      <c r="H26" s="50"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
       <c r="I26" s="3"/>
       <c r="J26" s="4"/>
     </row>
     <row r="27" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="50"/>
-      <c r="B27" s="24" t="s">
+      <c r="A27" s="27"/>
+      <c r="B27" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="C27" s="25" t="s">
+      <c r="C27" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="D27" s="25" t="s">
+      <c r="D27" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="E27" s="41" t="s">
+      <c r="E27" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="F27" s="25"/>
-      <c r="G27" s="50"/>
-      <c r="H27" s="50"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
       <c r="J27" s="4"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="50"/>
-      <c r="B28" s="27"/>
-      <c r="C28" s="28" t="s">
+      <c r="A28" s="27"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="D28" s="42" t="s">
+      <c r="D28" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="E28" s="43" t="s">
+      <c r="E28" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="F28" s="42"/>
-      <c r="G28" s="50"/>
-      <c r="H28" s="50"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="27"/>
       <c r="J28" s="4"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="50"/>
-      <c r="B29" s="27"/>
-      <c r="C29" s="44" t="s">
+      <c r="A29" s="27"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="D29" s="45"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="50"/>
-      <c r="H29" s="50"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
       <c r="J29" s="4"/>
     </row>
     <row r="30" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="50"/>
-      <c r="B30" s="47" t="s">
+      <c r="A30" s="27"/>
+      <c r="B30" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="C30" s="51" t="s">
+      <c r="C30" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="D30" s="25" t="s">
+      <c r="D30" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="E30" s="25" t="s">
+      <c r="E30" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="F30" s="25"/>
-      <c r="G30" s="50"/>
-      <c r="H30" s="50"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
       <c r="J30" s="4"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="50"/>
-      <c r="B31" s="27" t="s">
+      <c r="A31" s="27"/>
+      <c r="B31" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D31" s="11" t="s">
+      <c r="D31" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="E31" s="12" t="s">
+      <c r="E31" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F31" s="11"/>
-      <c r="G31" s="50"/>
-      <c r="H31" s="50"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
       <c r="J31" s="4"/>
       <c r="L31" s="5"/>
     </row>
     <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="50"/>
-      <c r="B32" s="27"/>
-      <c r="C32" s="25" t="s">
+      <c r="A32" s="27"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D32" s="25" t="s">
+      <c r="D32" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="E32" s="26" t="s">
+      <c r="E32" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="F32" s="25"/>
-      <c r="G32" s="50"/>
-      <c r="H32" s="50"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="27"/>
+      <c r="H32" s="27"/>
       <c r="J32" s="4"/>
     </row>
     <row r="33" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="40"/>
-      <c r="C33" s="11" t="s">
+      <c r="B33" s="30"/>
+      <c r="C33" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D33" s="11" t="s">
+      <c r="D33" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="E33" s="12" t="s">
+      <c r="E33" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="F33" s="11"/>
+      <c r="F33" s="10"/>
       <c r="H33" s="1"/>
     </row>
     <row r="34" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="24" t="s">
+      <c r="B34" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="C34" s="25" t="s">
+      <c r="C34" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D34" s="25" t="s">
+      <c r="D34" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="E34" s="25" t="s">
+      <c r="E34" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="F34" s="25"/>
+      <c r="F34" s="17"/>
     </row>
     <row r="35" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="27"/>
-      <c r="C35" s="11" t="s">
+      <c r="B35" s="29"/>
+      <c r="C35" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="D35" s="11" t="s">
+      <c r="D35" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="E35" s="11" t="s">
+      <c r="E35" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F35" s="48"/>
+      <c r="F35" s="26"/>
     </row>
     <row r="36" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="27"/>
-      <c r="C36" s="25" t="s">
+      <c r="B36" s="29"/>
+      <c r="C36" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="D36" s="25" t="s">
+      <c r="D36" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="E36" s="25" t="s">
+      <c r="E36" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="F36" s="25"/>
+      <c r="F36" s="17"/>
     </row>
     <row r="37" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="40"/>
-      <c r="C37" s="11" t="s">
+      <c r="B37" s="30"/>
+      <c r="C37" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="D37" s="11" t="s">
+      <c r="D37" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="E37" s="48" t="s">
+      <c r="E37" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="F37" s="11"/>
+      <c r="F37" s="10"/>
       <c r="J37" s="4"/>
     </row>
     <row r="38" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="47" t="s">
+      <c r="B38" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="C38" s="25" t="s">
+      <c r="C38" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D38" s="25" t="s">
+      <c r="D38" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="E38" s="25" t="s">
+      <c r="E38" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="F38" s="25"/>
+      <c r="F38" s="17"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B39" s="24" t="s">
+      <c r="B39" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="C39" s="28" t="s">
+      <c r="C39" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="D39" s="42" t="s">
+      <c r="D39" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="E39" s="42" t="s">
+      <c r="E39" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="F39" s="42"/>
+      <c r="F39" s="32"/>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B40" s="27"/>
-      <c r="C40" s="31" t="s">
+      <c r="B40" s="29"/>
+      <c r="C40" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="D40" s="49"/>
-      <c r="E40" s="49"/>
-      <c r="F40" s="49"/>
+      <c r="D40" s="33"/>
+      <c r="E40" s="33"/>
+      <c r="F40" s="33"/>
     </row>
     <row r="41" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="40"/>
-      <c r="C41" s="44" t="s">
+      <c r="B41" s="30"/>
+      <c r="C41" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="D41" s="45"/>
-      <c r="E41" s="45"/>
-      <c r="F41" s="45"/>
+      <c r="D41" s="34"/>
+      <c r="E41" s="34"/>
+      <c r="F41" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="D39:D41"/>
-    <mergeCell ref="E39:E41"/>
-    <mergeCell ref="F39:F41"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="D18:D23"/>
-    <mergeCell ref="E18:E23"/>
-    <mergeCell ref="F18:F23"/>
     <mergeCell ref="B27:B29"/>
     <mergeCell ref="D28:D29"/>
     <mergeCell ref="E28:E29"/>
@@ -1683,6 +1711,16 @@
     <mergeCell ref="F11:F12"/>
     <mergeCell ref="D15:D17"/>
     <mergeCell ref="E15:E17"/>
+    <mergeCell ref="F39:F41"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="D18:D23"/>
+    <mergeCell ref="E18:E23"/>
+    <mergeCell ref="F18:F23"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="E39:E41"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Change a component and redesign drills
The thermistor is sustituted by a connector in order to have no wirings
in the PCB. The thermistor has to be located near the battery.

Drills were redesign in orther to create a correct version to send to a
PCB manufacturer.
</commit_message>
<xml_diff>
--- a/fuel-gauge/Bill-Of-Materials-fuel-gauge.xlsx
+++ b/fuel-gauge/Bill-Of-Materials-fuel-gauge.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="99">
   <si>
     <t>C2</t>
   </si>
@@ -51,9 +51,6 @@
     <t>R4</t>
   </si>
   <si>
-    <t>TH1</t>
-  </si>
-  <si>
     <t>IC</t>
   </si>
   <si>
@@ -105,9 +102,6 @@
     <t xml:space="preserve">652-CR0805JW-101ELF </t>
   </si>
   <si>
-    <t xml:space="preserve">954-103AT-2 </t>
-  </si>
-  <si>
     <t xml:space="preserve">595-BQ34Z100PWR-G1 </t>
   </si>
   <si>
@@ -258,12 +252,6 @@
     <t>D3</t>
   </si>
   <si>
-    <t>THERMISTOR</t>
-  </si>
-  <si>
-    <t>10 KΩ</t>
-  </si>
-  <si>
     <t>BSS84</t>
   </si>
   <si>
@@ -319,6 +307,12 @@
   </si>
   <si>
     <t>P3</t>
+  </si>
+  <si>
+    <t>P4</t>
+  </si>
+  <si>
+    <t>483-8461</t>
   </si>
 </sst>
 </file>
@@ -362,7 +356,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -381,8 +375,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -572,12 +572,64 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -654,40 +706,34 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -708,22 +754,19 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -735,13 +778,40 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1048,8 +1118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1071,632 +1141,634 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="27"/>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
+      <c r="A1" s="26"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
       <c r="J1" s="4"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="27"/>
+      <c r="A2" s="26"/>
       <c r="B2" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="E2" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="F2" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="J2" s="4"/>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="26"/>
+      <c r="B3" s="33" t="s">
         <v>36</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="J2" s="4"/>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="27"/>
-      <c r="B3" s="46" t="s">
-        <v>38</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F3" s="10"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
       <c r="J3" s="4"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="27"/>
-      <c r="B4" s="47"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="34"/>
       <c r="C4" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="38" t="s">
+      <c r="D4" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="36"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="J4" s="4"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="26"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="37"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="26"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="38"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="J4" s="4"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
-      <c r="B5" s="47"/>
-      <c r="C5" s="13" t="s">
+      <c r="D6" s="37"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="J6" s="4"/>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="26"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="39"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-      <c r="J5" s="4"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="27"/>
-      <c r="B6" s="47"/>
-      <c r="C6" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="39"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
-      <c r="J6" s="4"/>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="27"/>
-      <c r="B7" s="47"/>
-      <c r="C7" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" s="40"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
       <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="27"/>
-      <c r="B8" s="48"/>
+      <c r="A8" s="26"/>
+      <c r="B8" s="35"/>
       <c r="C8" s="10" t="s">
         <v>1</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F8" s="10"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
       <c r="J8" s="4"/>
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="27"/>
-      <c r="B9" s="31" t="s">
-        <v>45</v>
+      <c r="A9" s="26"/>
+      <c r="B9" s="27" t="s">
+        <v>43</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="17"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="J9" s="4"/>
+    </row>
+    <row r="10" spans="1:10" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="26"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="D10" s="10" t="s">
         <v>47</v>
-      </c>
-      <c r="F9" s="17"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-      <c r="J9" s="4"/>
-    </row>
-    <row r="10" spans="1:10" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="27"/>
-      <c r="B10" s="29"/>
-      <c r="C10" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>49</v>
       </c>
       <c r="E10" s="11"/>
       <c r="F10" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="J10" s="6"/>
+    </row>
+    <row r="11" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="26"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="J10" s="6"/>
-    </row>
-    <row r="11" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="27"/>
-      <c r="B11" s="29"/>
-      <c r="C11" s="12" t="s">
+      <c r="E11" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="36"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="J11" s="6"/>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="26"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="E11" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="38"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="J11" s="6"/>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="27"/>
-      <c r="B12" s="29"/>
-      <c r="C12" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12" s="40"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
       <c r="J12" s="4"/>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="27"/>
-      <c r="B13" s="29"/>
+      <c r="A13" s="26"/>
+      <c r="B13" s="28"/>
       <c r="C13" s="10" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F13" s="10"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
       <c r="J13" s="4"/>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="27"/>
-      <c r="B14" s="29"/>
+      <c r="A14" s="26"/>
+      <c r="B14" s="28"/>
       <c r="C14" s="17" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="17"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="J14" s="4"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="26"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="D15" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="F14" s="17"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-      <c r="J14" s="4"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="27"/>
-      <c r="B15" s="29"/>
-      <c r="C15" s="19" t="s">
+      <c r="E15" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="44"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="J15" s="4"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="26"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="35" t="s">
+      <c r="D16" s="45"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+      <c r="J16" s="4"/>
+    </row>
+    <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="26"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="E15" s="50" t="s">
-        <v>23</v>
-      </c>
-      <c r="F15" s="35"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="27"/>
-      <c r="J15" s="4"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="27"/>
-      <c r="B16" s="29"/>
-      <c r="C16" s="20" t="s">
+      <c r="D17" s="46"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+      <c r="J17" s="4"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="26"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="D16" s="36"/>
-      <c r="E16" s="51"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
-      <c r="J16" s="4"/>
-    </row>
-    <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="27"/>
-      <c r="B17" s="29"/>
-      <c r="C17" s="21" t="s">
+      <c r="D18" s="50" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="37"/>
-      <c r="E17" s="52"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="27"/>
-      <c r="J17" s="4"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="27"/>
-      <c r="B18" s="49"/>
-      <c r="C18" s="22" t="s">
+      <c r="E18" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="36"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
+      <c r="J18" s="4"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="26"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="54" t="s">
+      <c r="D19" s="51"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="J19" s="4"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="26"/>
+      <c r="B20" s="42"/>
+      <c r="C20" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="E18" s="41" t="s">
-        <v>28</v>
-      </c>
-      <c r="F18" s="38"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="27"/>
-      <c r="J18" s="4"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="27"/>
-      <c r="B19" s="49"/>
-      <c r="C19" s="14" t="s">
+      <c r="D20" s="51"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="26"/>
+      <c r="J20" s="4"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="26"/>
+      <c r="B21" s="42"/>
+      <c r="C21" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="D19" s="53"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="27"/>
-      <c r="J19" s="4"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="27"/>
-      <c r="B20" s="49"/>
-      <c r="C20" s="14" t="s">
+      <c r="D21" s="51"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="J21" s="4"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="26"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="D20" s="53"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="39"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
-      <c r="J20" s="4"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="27"/>
-      <c r="B21" s="49"/>
-      <c r="C21" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="D21" s="53"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="39"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
-      <c r="J21" s="4"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="27"/>
-      <c r="B22" s="49"/>
-      <c r="C22" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="D22" s="53"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="27"/>
+      <c r="D22" s="51"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26"/>
       <c r="J22" s="4"/>
       <c r="L22" s="5"/>
     </row>
     <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="27"/>
-      <c r="B23" s="49"/>
+      <c r="A23" s="26"/>
+      <c r="B23" s="42"/>
       <c r="C23" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" s="52"/>
+      <c r="E23" s="41"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
+      <c r="J23" s="4"/>
+    </row>
+    <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="26"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="D23" s="55"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="40"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="27"/>
-      <c r="J23" s="4"/>
-    </row>
-    <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="27"/>
-      <c r="B24" s="29"/>
-      <c r="C24" s="10" t="s">
+      <c r="E24" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="F24" s="10"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
+      <c r="J24" s="4"/>
+    </row>
+    <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="26"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="D25" s="17" t="s">
         <v>70</v>
-      </c>
-      <c r="F24" s="10"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="27"/>
-      <c r="J24" s="4"/>
-    </row>
-    <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="27"/>
-      <c r="B25" s="29"/>
-      <c r="C25" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>72</v>
       </c>
       <c r="E25" s="18"/>
       <c r="F25" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="G25" s="27"/>
-      <c r="H25" s="27"/>
+        <v>71</v>
+      </c>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
       <c r="J25" s="4"/>
       <c r="M25" s="7"/>
     </row>
     <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="27"/>
-      <c r="B26" s="30"/>
+      <c r="A26" s="26"/>
+      <c r="B26" s="43"/>
       <c r="C26" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F26" s="10"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="27"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
       <c r="I26" s="3"/>
       <c r="J26" s="4"/>
     </row>
     <row r="27" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="27"/>
-      <c r="B27" s="31" t="s">
-        <v>75</v>
+      <c r="A27" s="26"/>
+      <c r="B27" s="27" t="s">
+        <v>73</v>
       </c>
       <c r="C27" s="17" t="s">
         <v>3</v>
       </c>
       <c r="D27" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="E27" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="F27" s="17"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="26"/>
+      <c r="J27" s="4"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="26"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="D28" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="E27" s="23" t="s">
+      <c r="E28" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" s="29"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="26"/>
+      <c r="J28" s="4"/>
+    </row>
+    <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="26"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="D29" s="30"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="J29" s="4"/>
+    </row>
+    <row r="30" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="26"/>
+      <c r="B30" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F30" s="17"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="J30" s="4"/>
+      <c r="L30" s="5"/>
+    </row>
+    <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="26"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="57" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="57" t="s">
+        <v>79</v>
+      </c>
+      <c r="E31" s="58" t="s">
+        <v>80</v>
+      </c>
+      <c r="F31" s="57"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="26"/>
+      <c r="J31" s="4"/>
+    </row>
+    <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="43"/>
+      <c r="C32" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="E32" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="F32" s="17"/>
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="57" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" s="57" t="s">
+        <v>83</v>
+      </c>
+      <c r="E33" s="57" t="s">
+        <v>23</v>
+      </c>
+      <c r="F33" s="57"/>
+    </row>
+    <row r="34" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="28"/>
+      <c r="C34" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="D34" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="E34" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="F34" s="53"/>
+    </row>
+    <row r="35" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="28"/>
+      <c r="C35" s="57" t="s">
+        <v>86</v>
+      </c>
+      <c r="D35" s="57" t="s">
+        <v>87</v>
+      </c>
+      <c r="E35" s="57" t="s">
+        <v>30</v>
+      </c>
+      <c r="F35" s="57"/>
+    </row>
+    <row r="36" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="43"/>
+      <c r="C36" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="E36" s="53" t="s">
+        <v>28</v>
+      </c>
+      <c r="F36" s="17"/>
+      <c r="J36" s="4"/>
+    </row>
+    <row r="37" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="C37" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" s="57" t="s">
+        <v>91</v>
+      </c>
+      <c r="E37" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="F37" s="57"/>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B38" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="C38" s="54" t="s">
+        <v>93</v>
+      </c>
+      <c r="D38" s="36" t="s">
+        <v>94</v>
+      </c>
+      <c r="E38" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="F27" s="17"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="27"/>
-      <c r="J27" s="4"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="27"/>
-      <c r="B28" s="29"/>
-      <c r="C28" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="D28" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="E28" s="44" t="s">
-        <v>17</v>
-      </c>
-      <c r="F28" s="32"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="27"/>
-      <c r="J28" s="4"/>
-    </row>
-    <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="27"/>
-      <c r="B29" s="29"/>
-      <c r="C29" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="D29" s="34"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="34"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="J29" s="4"/>
-    </row>
-    <row r="30" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="27"/>
-      <c r="B30" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="C30" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="E30" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="F30" s="17"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="J30" s="4"/>
-    </row>
-    <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="27"/>
-      <c r="B31" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="E31" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F31" s="10"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="27"/>
-      <c r="J31" s="4"/>
-      <c r="L31" s="5"/>
-    </row>
-    <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="27"/>
-      <c r="B32" s="29"/>
-      <c r="C32" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="E32" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="F32" s="17"/>
-      <c r="G32" s="27"/>
-      <c r="H32" s="27"/>
-      <c r="J32" s="4"/>
-    </row>
-    <row r="33" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="30"/>
-      <c r="C33" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="E33" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="F33" s="10"/>
-      <c r="H33" s="1"/>
-    </row>
-    <row r="34" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="C34" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D34" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="E34" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="F34" s="17"/>
-    </row>
-    <row r="35" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="29"/>
-      <c r="C35" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="D35" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="E35" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F35" s="26"/>
-    </row>
-    <row r="36" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="29"/>
-      <c r="C36" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="D36" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="E36" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="F36" s="17"/>
-    </row>
-    <row r="37" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="30"/>
-      <c r="C37" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="D37" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="E37" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="F37" s="10"/>
-      <c r="J37" s="4"/>
-    </row>
-    <row r="38" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="C38" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D38" s="17" t="s">
+      <c r="F38" s="50"/>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B39" s="28"/>
+      <c r="C39" s="55" t="s">
         <v>95</v>
       </c>
-      <c r="E38" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="F38" s="17"/>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B39" s="31" t="s">
+      <c r="D39" s="37"/>
+      <c r="E39" s="37"/>
+      <c r="F39" s="51"/>
+    </row>
+    <row r="40" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="28"/>
+      <c r="C40" s="56" t="s">
         <v>96</v>
       </c>
-      <c r="C39" s="19" t="s">
+      <c r="D40" s="38"/>
+      <c r="E40" s="38"/>
+      <c r="F40" s="52"/>
+    </row>
+    <row r="41" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="43"/>
+      <c r="C41" s="59" t="s">
         <v>97</v>
       </c>
-      <c r="D39" s="32" t="s">
+      <c r="D41" s="60"/>
+      <c r="E41" s="60"/>
+      <c r="F41" s="61" t="s">
         <v>98</v>
       </c>
-      <c r="E39" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="F39" s="32"/>
-    </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B40" s="29"/>
-      <c r="C40" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="D40" s="33"/>
-      <c r="E40" s="33"/>
-      <c r="F40" s="33"/>
-    </row>
-    <row r="41" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="30"/>
-      <c r="C41" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="D41" s="34"/>
-      <c r="E41" s="34"/>
-      <c r="F41" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="B33:B36"/>
+    <mergeCell ref="D38:D40"/>
+    <mergeCell ref="E38:E40"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="F38:F40"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="D18:D23"/>
+    <mergeCell ref="E18:E23"/>
+    <mergeCell ref="F18:F23"/>
     <mergeCell ref="B27:B29"/>
     <mergeCell ref="D28:D29"/>
     <mergeCell ref="E28:E29"/>
@@ -1711,16 +1783,6 @@
     <mergeCell ref="F11:F12"/>
     <mergeCell ref="D15:D17"/>
     <mergeCell ref="E15:E17"/>
-    <mergeCell ref="F39:F41"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="D18:D23"/>
-    <mergeCell ref="E18:E23"/>
-    <mergeCell ref="F18:F23"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="D39:D41"/>
-    <mergeCell ref="E39:E41"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Update the v2.0 of the fuel gauge PCB
Include the Bill of Materials (BOM) with all the components

Include the new footprint of the mounting hole
</commit_message>
<xml_diff>
--- a/fuel-gauge/Bill-Of-Materials-fuel-gauge.xlsx
+++ b/fuel-gauge/Bill-Of-Materials-fuel-gauge.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="585" windowWidth="14805" windowHeight="7530"/>
+    <workbookView xWindow="240" yWindow="645" windowWidth="14805" windowHeight="7470"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -177,9 +177,6 @@
     <t>165 kΩ</t>
   </si>
   <si>
-    <t>0.01 Ω</t>
-  </si>
-  <si>
     <t xml:space="preserve">71-WSL2010R0100FEA18 </t>
   </si>
   <si>
@@ -313,6 +310,9 @@
   </si>
   <si>
     <t>483-8461</t>
+  </si>
+  <si>
+    <t>0.01 Ω - 1%</t>
   </si>
 </sst>
 </file>
@@ -709,11 +709,77 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -736,37 +802,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -777,42 +813,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1119,7 +1119,7 @@
   <dimension ref="A1:M41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1127,7 +1127,7 @@
     <col min="1" max="1" width="6.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="15.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="26.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -1174,7 +1174,7 @@
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26"/>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="55" t="s">
         <v>36</v>
       </c>
       <c r="C3" s="10" t="s">
@@ -1193,63 +1193,63 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="26"/>
-      <c r="B4" s="34"/>
+      <c r="B4" s="56"/>
       <c r="C4" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="36" t="s">
+      <c r="D4" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="39" t="s">
+      <c r="E4" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="36"/>
+      <c r="F4" s="39"/>
       <c r="G4" s="26"/>
       <c r="H4" s="26"/>
       <c r="J4" s="4"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="26"/>
-      <c r="B5" s="34"/>
+      <c r="B5" s="56"/>
       <c r="C5" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="37"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="37"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="40"/>
       <c r="G5" s="26"/>
       <c r="H5" s="26"/>
       <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="26"/>
-      <c r="B6" s="34"/>
+      <c r="B6" s="56"/>
       <c r="C6" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="37"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="37"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="40"/>
       <c r="G6" s="26"/>
       <c r="H6" s="26"/>
       <c r="J6" s="4"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="26"/>
-      <c r="B7" s="34"/>
+      <c r="B7" s="56"/>
       <c r="C7" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="38"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="38"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="26"/>
       <c r="H7" s="26"/>
       <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="26"/>
-      <c r="B8" s="35"/>
+      <c r="B8" s="57"/>
       <c r="C8" s="10" t="s">
         <v>1</v>
       </c>
@@ -1266,7 +1266,7 @@
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="26"/>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="36" t="s">
         <v>43</v>
       </c>
       <c r="C9" s="17" t="s">
@@ -1285,7 +1285,7 @@
     </row>
     <row r="10" spans="1:10" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="26"/>
-      <c r="B10" s="28"/>
+      <c r="B10" s="37"/>
       <c r="C10" s="10" t="s">
         <v>46</v>
       </c>
@@ -1302,37 +1302,37 @@
     </row>
     <row r="11" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="26"/>
-      <c r="B11" s="28"/>
+      <c r="B11" s="37"/>
       <c r="C11" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="36" t="s">
+      <c r="D11" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="E11" s="39" t="s">
+      <c r="E11" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="36"/>
+      <c r="F11" s="39"/>
       <c r="G11" s="26"/>
       <c r="H11" s="26"/>
       <c r="J11" s="6"/>
     </row>
     <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="26"/>
-      <c r="B12" s="28"/>
+      <c r="B12" s="37"/>
       <c r="C12" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="38"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="38"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="41"/>
       <c r="G12" s="26"/>
       <c r="H12" s="26"/>
       <c r="J12" s="4"/>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="26"/>
-      <c r="B13" s="28"/>
+      <c r="B13" s="37"/>
       <c r="C13" s="10" t="s">
         <v>10</v>
       </c>
@@ -1349,15 +1349,15 @@
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="26"/>
-      <c r="B14" s="28"/>
+      <c r="B14" s="37"/>
       <c r="C14" s="17" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="E14" s="18" t="s">
         <v>53</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>54</v>
       </c>
       <c r="F14" s="17"/>
       <c r="G14" s="26"/>
@@ -1366,112 +1366,112 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="26"/>
-      <c r="B15" s="28"/>
+      <c r="B15" s="37"/>
       <c r="C15" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="45" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="44" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" s="47" t="s">
+      <c r="E15" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="44"/>
+      <c r="F15" s="45"/>
       <c r="G15" s="26"/>
       <c r="H15" s="26"/>
       <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="26"/>
-      <c r="B16" s="28"/>
+      <c r="B16" s="37"/>
       <c r="C16" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="D16" s="45"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="45"/>
+        <v>56</v>
+      </c>
+      <c r="D16" s="46"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="46"/>
       <c r="G16" s="26"/>
       <c r="H16" s="26"/>
       <c r="J16" s="4"/>
     </row>
     <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="26"/>
-      <c r="B17" s="28"/>
+      <c r="B17" s="37"/>
       <c r="C17" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="D17" s="46"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="46"/>
+        <v>57</v>
+      </c>
+      <c r="D17" s="47"/>
+      <c r="E17" s="61"/>
+      <c r="F17" s="47"/>
       <c r="G17" s="26"/>
       <c r="H17" s="26"/>
       <c r="J17" s="4"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="26"/>
-      <c r="B18" s="42"/>
+      <c r="B18" s="58"/>
       <c r="C18" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="D18" s="50" t="s">
-        <v>60</v>
-      </c>
-      <c r="E18" s="39" t="s">
+      <c r="E18" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="F18" s="36"/>
+      <c r="F18" s="39"/>
       <c r="G18" s="26"/>
       <c r="H18" s="26"/>
       <c r="J18" s="4"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="26"/>
-      <c r="B19" s="42"/>
+      <c r="B19" s="58"/>
       <c r="C19" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="D19" s="51"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="37"/>
+        <v>60</v>
+      </c>
+      <c r="D19" s="43"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="40"/>
       <c r="G19" s="26"/>
       <c r="H19" s="26"/>
       <c r="J19" s="4"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="26"/>
-      <c r="B20" s="42"/>
+      <c r="B20" s="58"/>
       <c r="C20" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="D20" s="51"/>
-      <c r="E20" s="40"/>
-      <c r="F20" s="37"/>
+        <v>61</v>
+      </c>
+      <c r="D20" s="43"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="40"/>
       <c r="G20" s="26"/>
       <c r="H20" s="26"/>
       <c r="J20" s="4"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="26"/>
-      <c r="B21" s="42"/>
+      <c r="B21" s="58"/>
       <c r="C21" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="D21" s="51"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="37"/>
+        <v>62</v>
+      </c>
+      <c r="D21" s="43"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="40"/>
       <c r="G21" s="26"/>
       <c r="H21" s="26"/>
       <c r="J21" s="4"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="26"/>
-      <c r="B22" s="42"/>
+      <c r="B22" s="58"/>
       <c r="C22" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="D22" s="51"/>
-      <c r="E22" s="40"/>
-      <c r="F22" s="37"/>
+        <v>63</v>
+      </c>
+      <c r="D22" s="43"/>
+      <c r="E22" s="49"/>
+      <c r="F22" s="40"/>
       <c r="G22" s="26"/>
       <c r="H22" s="26"/>
       <c r="J22" s="4"/>
@@ -1479,28 +1479,28 @@
     </row>
     <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="26"/>
-      <c r="B23" s="42"/>
+      <c r="B23" s="58"/>
       <c r="C23" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="D23" s="52"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="38"/>
+        <v>64</v>
+      </c>
+      <c r="D23" s="44"/>
+      <c r="E23" s="50"/>
+      <c r="F23" s="41"/>
       <c r="G23" s="26"/>
       <c r="H23" s="26"/>
       <c r="J23" s="4"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="26"/>
-      <c r="B24" s="28"/>
+      <c r="B24" s="37"/>
       <c r="C24" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="E24" s="10" t="s">
         <v>67</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>68</v>
       </c>
       <c r="F24" s="10"/>
       <c r="G24" s="26"/>
@@ -1509,16 +1509,16 @@
     </row>
     <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="26"/>
-      <c r="B25" s="28"/>
+      <c r="B25" s="37"/>
       <c r="C25" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" s="17" t="s">
         <v>69</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>70</v>
       </c>
       <c r="E25" s="18"/>
       <c r="F25" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G25" s="26"/>
       <c r="H25" s="26"/>
@@ -1527,12 +1527,12 @@
     </row>
     <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="26"/>
-      <c r="B26" s="43"/>
+      <c r="B26" s="38"/>
       <c r="C26" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E26" s="10" t="s">
         <v>24</v>
@@ -1545,14 +1545,14 @@
     </row>
     <row r="27" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="26"/>
-      <c r="B27" s="27" t="s">
-        <v>73</v>
+      <c r="B27" s="36" t="s">
+        <v>72</v>
       </c>
       <c r="C27" s="17" t="s">
         <v>3</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E27" s="23" t="s">
         <v>17</v>
@@ -1564,44 +1564,44 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="26"/>
-      <c r="B28" s="28"/>
+      <c r="B28" s="37"/>
       <c r="C28" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28" s="51" t="s">
         <v>75</v>
       </c>
-      <c r="D28" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="E28" s="31" t="s">
+      <c r="E28" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="F28" s="29"/>
+      <c r="F28" s="51"/>
       <c r="G28" s="26"/>
       <c r="H28" s="26"/>
       <c r="J28" s="4"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="26"/>
-      <c r="B29" s="28"/>
+      <c r="B29" s="37"/>
       <c r="C29" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="D29" s="30"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="30"/>
+        <v>76</v>
+      </c>
+      <c r="D29" s="52"/>
+      <c r="E29" s="54"/>
+      <c r="F29" s="52"/>
       <c r="G29" s="26"/>
       <c r="H29" s="26"/>
       <c r="J29" s="4"/>
     </row>
     <row r="30" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="26"/>
-      <c r="B30" s="27" t="s">
+      <c r="B30" s="36" t="s">
         <v>4</v>
       </c>
       <c r="C30" s="17" t="s">
         <v>7</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E30" s="18" t="s">
         <v>20</v>
@@ -1614,85 +1614,85 @@
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="26"/>
-      <c r="B31" s="28"/>
-      <c r="C31" s="57" t="s">
+      <c r="B31" s="37"/>
+      <c r="C31" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="D31" s="57" t="s">
+      <c r="D31" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="E31" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="E31" s="58" t="s">
-        <v>80</v>
-      </c>
-      <c r="F31" s="57"/>
+      <c r="F31" s="31"/>
       <c r="G31" s="26"/>
       <c r="H31" s="26"/>
       <c r="J31" s="4"/>
     </row>
     <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="43"/>
+      <c r="B32" s="38"/>
       <c r="C32" s="17" t="s">
         <v>5</v>
       </c>
       <c r="D32" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="E32" s="18" t="s">
         <v>81</v>
-      </c>
-      <c r="E32" s="18" t="s">
-        <v>82</v>
       </c>
       <c r="F32" s="17"/>
       <c r="H32" s="1"/>
     </row>
     <row r="33" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="27" t="s">
+      <c r="B33" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="C33" s="57" t="s">
+      <c r="C33" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="D33" s="57" t="s">
+      <c r="D33" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="E33" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="F33" s="31"/>
+    </row>
+    <row r="34" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="37"/>
+      <c r="C34" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="E33" s="57" t="s">
-        <v>23</v>
-      </c>
-      <c r="F33" s="57"/>
-    </row>
-    <row r="34" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="28"/>
-      <c r="C34" s="17" t="s">
+      <c r="D34" s="17" t="s">
         <v>84</v>
-      </c>
-      <c r="D34" s="17" t="s">
-        <v>85</v>
       </c>
       <c r="E34" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="F34" s="53"/>
+      <c r="F34" s="27"/>
     </row>
     <row r="35" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="28"/>
-      <c r="C35" s="57" t="s">
+      <c r="B35" s="37"/>
+      <c r="C35" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="D35" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="D35" s="57" t="s">
+      <c r="E35" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="F35" s="31"/>
+    </row>
+    <row r="36" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="38"/>
+      <c r="C36" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="E35" s="57" t="s">
-        <v>30</v>
-      </c>
-      <c r="F35" s="57"/>
-    </row>
-    <row r="36" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="43"/>
-      <c r="C36" s="17" t="s">
+      <c r="D36" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="D36" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="E36" s="53" t="s">
+      <c r="E36" s="27" t="s">
         <v>28</v>
       </c>
       <c r="F36" s="17"/>
@@ -1700,75 +1700,65 @@
     </row>
     <row r="37" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C37" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="C37" s="57" t="s">
-        <v>13</v>
-      </c>
-      <c r="D37" s="57" t="s">
+      <c r="E37" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="F37" s="31"/>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B38" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="E37" s="57" t="s">
-        <v>29</v>
-      </c>
-      <c r="F37" s="57"/>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B38" s="27" t="s">
+      <c r="C38" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="C38" s="54" t="s">
+      <c r="D38" s="39" t="s">
         <v>93</v>
       </c>
-      <c r="D38" s="36" t="s">
+      <c r="E38" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="F38" s="42"/>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B39" s="37"/>
+      <c r="C39" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="E38" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="F38" s="50"/>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B39" s="28"/>
-      <c r="C39" s="55" t="s">
+      <c r="D39" s="40"/>
+      <c r="E39" s="40"/>
+      <c r="F39" s="43"/>
+    </row>
+    <row r="40" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="37"/>
+      <c r="C40" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="D39" s="37"/>
-      <c r="E39" s="37"/>
-      <c r="F39" s="51"/>
-    </row>
-    <row r="40" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="28"/>
-      <c r="C40" s="56" t="s">
+      <c r="D40" s="41"/>
+      <c r="E40" s="41"/>
+      <c r="F40" s="44"/>
+    </row>
+    <row r="41" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="38"/>
+      <c r="C41" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="D40" s="38"/>
-      <c r="E40" s="38"/>
-      <c r="F40" s="52"/>
-    </row>
-    <row r="41" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="43"/>
-      <c r="C41" s="59" t="s">
+      <c r="D41" s="34"/>
+      <c r="E41" s="34"/>
+      <c r="F41" s="35" t="s">
         <v>97</v>
-      </c>
-      <c r="D41" s="60"/>
-      <c r="E41" s="60"/>
-      <c r="F41" s="61" t="s">
-        <v>98</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="B33:B36"/>
-    <mergeCell ref="D38:D40"/>
-    <mergeCell ref="E38:E40"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="F38:F40"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="D18:D23"/>
-    <mergeCell ref="E18:E23"/>
-    <mergeCell ref="F18:F23"/>
     <mergeCell ref="B27:B29"/>
     <mergeCell ref="D28:D29"/>
     <mergeCell ref="E28:E29"/>
@@ -1783,6 +1773,16 @@
     <mergeCell ref="F11:F12"/>
     <mergeCell ref="D15:D17"/>
     <mergeCell ref="E15:E17"/>
+    <mergeCell ref="F38:F40"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="D18:D23"/>
+    <mergeCell ref="E18:E23"/>
+    <mergeCell ref="F18:F23"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="B33:B36"/>
+    <mergeCell ref="D38:D40"/>
+    <mergeCell ref="E38:E40"/>
+    <mergeCell ref="B38:B41"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>

</xml_diff>